<commit_message>
Added a write method for the excel sheet
</commit_message>
<xml_diff>
--- a/CompetitionReader/competitions.xlsx
+++ b/CompetitionReader/competitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Workspace\Java\CompetitionReader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\KFUPM Faculty\211\SWE206\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF49C3F-47AC-4B66-B4B0-8A2DCCECB397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F372ACD-8F1B-4EFA-AC39-677F06B479B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1500" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{54FEB0A3-0501-489B-8C15-4473C17019CE}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" activeTab="1" xr2:uid="{54FEB0A3-0501-489B-8C15-4473C17019CE}"/>
   </bookViews>
   <sheets>
     <sheet name="STC &amp; Nokia" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>team</t>
   </si>
@@ -122,12 +122,6 @@
   </si>
   <si>
     <t>CyberuHub</t>
-  </si>
-  <si>
-    <t>competition name</t>
-  </si>
-  <si>
-    <t>Competition link</t>
   </si>
 </sst>
 </file>
@@ -658,7 +652,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +665,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
@@ -679,7 +673,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -710,7 +704,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
         <v>222253860</v>
@@ -727,7 +721,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1">
         <v>222256560</v>
@@ -744,7 +738,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
         <v>222279260</v>
@@ -761,7 +755,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3">
         <v>222256700</v>

</xml_diff>